<commit_message>
fix: Dynamic model_id in schema UUIDs for Simple format
Bug: Schema UUIDs were always using hardcoded 0004 instead of actual model_id
from the Excel schema.

Root Cause: unified-schema-sync.ts was regenerating UUIDs with
buildSchemaUuidV2(field_id) instead of using the pre-generated UUID
from schema.qdrant_id.

Changes:
- Add buildSchemaUuidV2Simple(fieldId, modelId) function in uuid-v2.ts
- Update simple-schema-converter.ts to use new function with dynamic model_id
- Update generateSemanticText() to include FK Qdrant ID
- Fix unified-schema-sync.ts to use schema.qdrant_id directly
- Update sample schema files with proper model_id structure
- Add utility scripts for collection management and verification

UUID Format: 00000003-{model_id}-0000-0000-{field_id}
Example: customer field (model_id=2) → 00000003-0002-0000-0000-000000000201

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/samples/SAMPLE_payload_config.xlsx
+++ b/samples/SAMPLE_payload_config.xlsx
@@ -1,41 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KasunJ\MCP\Nexsus1\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF2E9D-AB29-4185-82DC-8B3209905958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+  <si>
+    <t>Field_ID</t>
+  </si>
+  <si>
+    <t>Model_ID</t>
+  </si>
+  <si>
+    <t>Model_Name</t>
+  </si>
+  <si>
+    <t>Field_Name</t>
+  </si>
+  <si>
+    <t>Field_Label</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>country_id</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>created_date</t>
+  </si>
+  <si>
+    <t>Created Date</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>Field_Type</t>
+  </si>
+  <si>
+    <t>Stored</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FK location field model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FK location field model id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FK location record Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Qdrant ID for FK</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +150,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,155 +500,422 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Field_ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Model_ID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Model_Name</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Field_Name</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Field_Label</v>
-      </c>
-      <c r="F1" t="str">
-        <v>payload</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="str">
-        <v>customer</v>
-      </c>
-      <c r="D2" t="str">
-        <v>id</v>
-      </c>
-      <c r="E2" t="str">
-        <v>ID</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>202</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="str">
-        <v>customer</v>
-      </c>
-      <c r="D3" t="str">
-        <v>name</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Customer Name</v>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>203</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>204</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>205</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>206</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>301</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="str">
-        <v>customer</v>
-      </c>
-      <c r="D4" t="str">
-        <v>email</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Email</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>302</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>103</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>104</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="str">
-        <v>customer</v>
-      </c>
-      <c r="D5" t="str">
-        <v>country_id</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Country</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <v>customer</v>
-      </c>
-      <c r="D6" t="str">
-        <v>status</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Status</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <v>customer</v>
-      </c>
-      <c r="D7" t="str">
-        <v>created_date</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Created Date</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>107</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>108</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>109</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>110</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>111</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D16:E16">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError sqref="A1:F1 C7:F7 C2:F2 C3:F3 C4:F4 C5:F5 C6:F6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Standardize FK column names with underscores
- Add underscore format as canonical FK column names:
  - FK_location_field_model
  - FK_location_field_model_id
  - FK_location_record_Id
  - Qdrant_ID_for_FK
- Update getFkField() to try underscore format first
- Add deprecated aliases for legacy space format
- Update types.ts with both formats for backward compatibility

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/samples/SAMPLE_payload_config.xlsx
+++ b/samples/SAMPLE_payload_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KasunJ\MCP\Nexsus1\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275E356E-DEC6-4E2C-B556-9B641E184E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC150DA3-D2BD-429B-8359-D40B340CD209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11712" yWindow="12852" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="55">
   <si>
     <t>Field_ID</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Classification</t>
   </si>
   <si>
-    <t>Master[EBITA]</t>
-  </si>
-  <si>
     <t>master</t>
   </si>
   <si>
@@ -183,6 +180,24 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Standard_costing</t>
+  </si>
+  <si>
+    <t>Account_Name</t>
+  </si>
+  <si>
+    <t>FK_location_field_model</t>
+  </si>
+  <si>
+    <t>FK_location_field_model_id</t>
+  </si>
+  <si>
+    <t>FK_location_record_Id</t>
+  </si>
+  <si>
+    <t>Qdrant_ID_for_FK</t>
   </si>
 </sst>
 </file>
@@ -587,21 +602,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
-    <col min="2" max="2" width="10.796875" customWidth="1"/>
-    <col min="3" max="3" width="13.8984375" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.296875" customWidth="1"/>
+    <col min="6" max="6" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -641,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -661,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
@@ -681,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -701,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>105</v>
       </c>
@@ -721,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>106</v>
       </c>
@@ -741,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>107</v>
       </c>
@@ -761,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>108</v>
       </c>
@@ -772,7 +787,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -781,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>109</v>
       </c>
@@ -792,7 +807,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -801,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>110</v>
       </c>
@@ -812,7 +827,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -821,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>111</v>
       </c>
@@ -832,7 +847,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -841,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>201</v>
       </c>
@@ -849,10 +864,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -861,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>202</v>
       </c>
@@ -869,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -881,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>203</v>
       </c>
@@ -889,7 +904,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -901,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>204</v>
       </c>
@@ -909,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -921,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>205</v>
       </c>
@@ -929,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -941,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>206</v>
       </c>
@@ -949,7 +964,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -961,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>207</v>
       </c>
@@ -969,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
         <v>19</v>
@@ -981,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>208</v>
       </c>
@@ -989,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -1001,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>209</v>
       </c>
@@ -1009,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -1021,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>210</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -1041,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>211</v>
       </c>
@@ -1049,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
@@ -1061,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>212</v>
       </c>
@@ -1069,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
@@ -1081,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>213</v>
       </c>
@@ -1089,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1101,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>214</v>
       </c>
@@ -1109,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -1121,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>215</v>
       </c>
@@ -1129,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -1141,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>216</v>
       </c>
@@ -1149,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -1161,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>217</v>
       </c>
@@ -1169,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>29</v>
@@ -1181,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>218</v>
       </c>
@@ -1189,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
         <v>30</v>
@@ -1201,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>219</v>
       </c>
@@ -1209,7 +1224,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
         <v>31</v>
@@ -1221,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>220</v>
       </c>
@@ -1229,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E32" t="s">
         <v>32</v>
@@ -1241,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>221</v>
       </c>
@@ -1249,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
         <v>33</v>
@@ -1261,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>222</v>
       </c>
@@ -1269,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
         <v>34</v>
@@ -1281,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>223</v>
       </c>
@@ -1289,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
@@ -1301,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>224</v>
       </c>
@@ -1309,7 +1324,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
         <v>36</v>
@@ -1321,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>225</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s">
         <v>37</v>
@@ -1341,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>226</v>
       </c>
@@ -1349,7 +1364,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
         <v>38</v>
@@ -1361,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>227</v>
       </c>
@@ -1369,7 +1384,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
         <v>39</v>
@@ -1381,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>301</v>
       </c>
@@ -1389,10 +1404,10 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" t="s">
         <v>40</v>
@@ -1401,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>302</v>
       </c>
@@ -1409,10 +1424,10 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
@@ -1421,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>303</v>
       </c>
@@ -1429,7 +1444,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
         <v>42</v>
@@ -1441,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>304</v>
       </c>
@@ -1449,7 +1464,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D43" t="s">
         <v>25</v>
@@ -1461,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>305</v>
       </c>
@@ -1469,7 +1484,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D44" t="s">
         <v>43</v>
@@ -1481,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>306</v>
       </c>
@@ -1489,19 +1504,19 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>307</v>
       </c>
@@ -1509,13 +1524,13 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>

</xml_diff>